<commit_message>
refactor: load current weather on index
</commit_message>
<xml_diff>
--- a/documents/Datentabelle.xlsx
+++ b/documents/Datentabelle.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://fhgraubuenden-my.sharepoint.com/personal/schallerjoel_fhgr_ch/Documents/Interaktive_Medien_IV/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Yannick/GitProjects/01_currentProjects/weathertunes/documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="143" documentId="13_ncr:1_{7513D333-58CD-084F-A01A-1F94D64D850B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7A2D5F91-A87E-44A3-9F9F-2F41E9F93596}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EEADE96-D3E9-6340-BE4D-A5BB15C46B9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{F4D6F30E-FA16-3844-B073-64C554E4A739}"/>
+    <workbookView xWindow="360" yWindow="840" windowWidth="30100" windowHeight="18080" xr2:uid="{F4D6F30E-FA16-3844-B073-64C554E4A739}"/>
   </bookViews>
   <sheets>
     <sheet name="Wetter" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="65">
   <si>
     <t>Beispiel-Datenpunkte</t>
   </si>
@@ -219,10 +219,20 @@
     <t>Min:  /  Max:</t>
   </si>
   <si>
-    <t>Codetabelle</t>
-  </si>
-  <si>
     <t>Min: 0 /  Max: 99</t>
+  </si>
+  <si>
+    <t>number</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>number
+Codetabelle</t>
+  </si>
+  <si>
+    <t>number (boolean)</t>
   </si>
 </sst>
 </file>
@@ -233,7 +243,7 @@
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -639,8 +649,8 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Link" xfId="1" builtinId="8"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -656,7 +666,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -975,13 +985,13 @@
   <dimension ref="A1:Z34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="66" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="J14" sqref="J14"/>
+      <selection pane="bottomRight" activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="25" customWidth="1"/>
     <col min="2" max="2" width="21.83203125" style="32" bestFit="1" customWidth="1"/>
@@ -989,7 +999,7 @@
     <col min="4" max="26" width="20.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" s="39" customFormat="1" ht="35" customHeight="1">
+    <row r="1" spans="1:26" s="39" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="15" t="s">
         <v>3</v>
       </c>
@@ -1039,7 +1049,7 @@
       <c r="Y1" s="38"/>
       <c r="Z1" s="38"/>
     </row>
-    <row r="2" spans="1:26" s="12" customFormat="1" ht="60" customHeight="1" thickBot="1">
+    <row r="2" spans="1:26" s="12" customFormat="1" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
         <v>2</v>
       </c>
@@ -1089,7 +1099,7 @@
       <c r="Y2" s="11"/>
       <c r="Z2" s="11"/>
     </row>
-    <row r="3" spans="1:26" s="6" customFormat="1" ht="28" customHeight="1">
+    <row r="3" spans="1:26" s="6" customFormat="1" ht="28" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="41" t="s">
         <v>0</v>
       </c>
@@ -1139,7 +1149,7 @@
       <c r="Y3" s="5"/>
       <c r="Z3" s="5"/>
     </row>
-    <row r="4" spans="1:26" s="6" customFormat="1" ht="28" customHeight="1">
+    <row r="4" spans="1:26" s="6" customFormat="1" ht="28" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="42"/>
       <c r="B4" s="21"/>
       <c r="C4" s="21"/>
@@ -1167,7 +1177,7 @@
       <c r="Y4" s="5"/>
       <c r="Z4" s="5"/>
     </row>
-    <row r="5" spans="1:26" s="6" customFormat="1" ht="28" customHeight="1">
+    <row r="5" spans="1:26" s="6" customFormat="1" ht="28" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="42"/>
       <c r="B5" s="21"/>
       <c r="C5" s="21"/>
@@ -1195,7 +1205,7 @@
       <c r="Y5" s="5"/>
       <c r="Z5" s="5"/>
     </row>
-    <row r="6" spans="1:26" s="6" customFormat="1" ht="28" customHeight="1">
+    <row r="6" spans="1:26" s="6" customFormat="1" ht="28" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="42"/>
       <c r="B6" s="21"/>
       <c r="C6" s="21"/>
@@ -1223,7 +1233,7 @@
       <c r="Y6" s="5"/>
       <c r="Z6" s="5"/>
     </row>
-    <row r="7" spans="1:26" s="6" customFormat="1" ht="28" customHeight="1">
+    <row r="7" spans="1:26" s="6" customFormat="1" ht="28" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="42"/>
       <c r="B7" s="21"/>
       <c r="C7" s="21"/>
@@ -1251,7 +1261,7 @@
       <c r="Y7" s="5"/>
       <c r="Z7" s="5"/>
     </row>
-    <row r="8" spans="1:26" s="6" customFormat="1" ht="28" customHeight="1">
+    <row r="8" spans="1:26" s="6" customFormat="1" ht="28" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="42"/>
       <c r="B8" s="21"/>
       <c r="C8" s="21"/>
@@ -1279,7 +1289,7 @@
       <c r="Y8" s="5"/>
       <c r="Z8" s="5"/>
     </row>
-    <row r="9" spans="1:26" s="6" customFormat="1" ht="28" customHeight="1">
+    <row r="9" spans="1:26" s="6" customFormat="1" ht="28" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="42"/>
       <c r="B9" s="21"/>
       <c r="C9" s="21"/>
@@ -1307,7 +1317,7 @@
       <c r="Y9" s="5"/>
       <c r="Z9" s="5"/>
     </row>
-    <row r="10" spans="1:26" s="6" customFormat="1" ht="28" customHeight="1">
+    <row r="10" spans="1:26" s="6" customFormat="1" ht="28" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="42"/>
       <c r="B10" s="21"/>
       <c r="C10" s="21"/>
@@ -1335,7 +1345,7 @@
       <c r="Y10" s="5"/>
       <c r="Z10" s="5"/>
     </row>
-    <row r="11" spans="1:26" s="6" customFormat="1" ht="28" customHeight="1">
+    <row r="11" spans="1:26" s="6" customFormat="1" ht="28" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="42"/>
       <c r="B11" s="21"/>
       <c r="C11" s="21"/>
@@ -1363,7 +1373,7 @@
       <c r="Y11" s="5"/>
       <c r="Z11" s="5"/>
     </row>
-    <row r="12" spans="1:26" s="8" customFormat="1" ht="28" customHeight="1" thickBot="1">
+    <row r="12" spans="1:26" s="8" customFormat="1" ht="28" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="43"/>
       <c r="B12" s="22"/>
       <c r="C12" s="22"/>
@@ -1391,22 +1401,40 @@
       <c r="Y12" s="7"/>
       <c r="Z12" s="7"/>
     </row>
-    <row r="13" spans="1:26" s="14" customFormat="1" ht="36" customHeight="1" thickBot="1">
+    <row r="13" spans="1:26" s="14" customFormat="1" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="B13" s="29"/>
-      <c r="C13" s="24"/>
-      <c r="D13" s="24"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
-      <c r="H13" s="13"/>
-      <c r="I13" s="13"/>
-      <c r="J13" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="K13" s="13"/>
+      <c r="B13" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="C13" s="24" t="s">
+        <v>61</v>
+      </c>
+      <c r="D13" s="24" t="s">
+        <v>61</v>
+      </c>
+      <c r="E13" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="F13" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="G13" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="H13" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="I13" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="J13" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="K13" s="13" t="s">
+        <v>61</v>
+      </c>
       <c r="L13" s="13"/>
       <c r="M13" s="13"/>
       <c r="N13" s="13"/>
@@ -1423,7 +1451,7 @@
       <c r="Y13" s="13"/>
       <c r="Z13" s="13"/>
     </row>
-    <row r="14" spans="1:26" s="4" customFormat="1" ht="89" customHeight="1" thickBot="1">
+    <row r="14" spans="1:26" s="4" customFormat="1" ht="89" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="18" t="s">
         <v>4</v>
       </c>
@@ -1452,7 +1480,7 @@
         <v>59</v>
       </c>
       <c r="J14" s="30" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K14" s="30" t="s">
         <v>59</v>
@@ -1473,11 +1501,11 @@
       <c r="Y14" s="3"/>
       <c r="Z14" s="3"/>
     </row>
-    <row r="15" spans="1:26" ht="36" customHeight="1" thickBot="1">
+    <row r="15" spans="1:26" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B15" s="31"/>
       <c r="C15"/>
     </row>
-    <row r="16" spans="1:26" s="20" customFormat="1" ht="36" customHeight="1" thickBot="1">
+    <row r="16" spans="1:26" s="20" customFormat="1" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="19" t="s">
         <v>5</v>
       </c>
@@ -1494,13 +1522,13 @@
       <c r="J16" s="45"/>
       <c r="K16" s="45"/>
     </row>
-    <row r="18" spans="2:3">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B18" s="35" t="s">
         <v>53</v>
       </c>
       <c r="C18" s="36"/>
     </row>
-    <row r="19" spans="2:3">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B19" s="35" t="s">
         <v>27</v>
       </c>
@@ -1508,7 +1536,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="2:3">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B20" s="36">
         <v>0</v>
       </c>
@@ -1516,7 +1544,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="21" spans="2:3">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B21" s="36" t="s">
         <v>30</v>
       </c>
@@ -1524,7 +1552,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="22" spans="2:3">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B22" s="36" t="s">
         <v>32</v>
       </c>
@@ -1532,7 +1560,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="23" spans="2:3">
+    <row r="23" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B23" s="36" t="s">
         <v>34</v>
       </c>
@@ -1540,7 +1568,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="24" spans="2:3">
+    <row r="24" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B24" s="36" t="s">
         <v>36</v>
       </c>
@@ -1548,7 +1576,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="25" spans="2:3">
+    <row r="25" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B25" s="36" t="s">
         <v>38</v>
       </c>
@@ -1556,7 +1584,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="26" spans="2:3">
+    <row r="26" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B26" s="36" t="s">
         <v>40</v>
       </c>
@@ -1564,7 +1592,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="27" spans="2:3">
+    <row r="27" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B27" s="36" t="s">
         <v>42</v>
       </c>
@@ -1572,7 +1600,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="28" spans="2:3">
+    <row r="28" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B28" s="36">
         <v>77</v>
       </c>
@@ -1580,7 +1608,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="29" spans="2:3">
+    <row r="29" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B29" s="36" t="s">
         <v>45</v>
       </c>
@@ -1588,7 +1616,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="30" spans="2:3">
+    <row r="30" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B30" s="36" t="s">
         <v>47</v>
       </c>
@@ -1596,7 +1624,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="31" spans="2:3">
+    <row r="31" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B31" s="36" t="s">
         <v>49</v>
       </c>
@@ -1604,7 +1632,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="32" spans="2:3">
+    <row r="32" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B32" s="36" t="s">
         <v>51</v>
       </c>
@@ -1612,7 +1640,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="34" spans="3:3">
+    <row r="34" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C34" s="40" t="s">
         <v>55</v>
       </c>
@@ -1640,7 +1668,7 @@
       <selection pane="bottomRight" activeCell="B1" sqref="B1:K1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="25" customWidth="1"/>
     <col min="2" max="2" width="20.83203125" style="32" customWidth="1"/>
@@ -1648,7 +1676,7 @@
     <col min="4" max="26" width="20.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" s="39" customFormat="1" ht="35" customHeight="1">
+    <row r="1" spans="1:26" s="39" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="15" t="s">
         <v>3</v>
       </c>
@@ -1678,7 +1706,7 @@
       <c r="Y1" s="38"/>
       <c r="Z1" s="38"/>
     </row>
-    <row r="2" spans="1:26" s="12" customFormat="1" ht="60" customHeight="1" thickBot="1">
+    <row r="2" spans="1:26" s="12" customFormat="1" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
         <v>2</v>
       </c>
@@ -1708,7 +1736,7 @@
       <c r="Y2" s="11"/>
       <c r="Z2" s="11"/>
     </row>
-    <row r="3" spans="1:26" s="6" customFormat="1" ht="28" customHeight="1">
+    <row r="3" spans="1:26" s="6" customFormat="1" ht="28" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="41" t="s">
         <v>0</v>
       </c>
@@ -1738,7 +1766,7 @@
       <c r="Y3" s="5"/>
       <c r="Z3" s="5"/>
     </row>
-    <row r="4" spans="1:26" s="6" customFormat="1" ht="28" customHeight="1">
+    <row r="4" spans="1:26" s="6" customFormat="1" ht="28" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="42"/>
       <c r="B4" s="21"/>
       <c r="C4" s="21"/>
@@ -1766,7 +1794,7 @@
       <c r="Y4" s="5"/>
       <c r="Z4" s="5"/>
     </row>
-    <row r="5" spans="1:26" s="6" customFormat="1" ht="28" customHeight="1">
+    <row r="5" spans="1:26" s="6" customFormat="1" ht="28" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="42"/>
       <c r="B5" s="21"/>
       <c r="C5" s="21"/>
@@ -1794,7 +1822,7 @@
       <c r="Y5" s="5"/>
       <c r="Z5" s="5"/>
     </row>
-    <row r="6" spans="1:26" s="6" customFormat="1" ht="28" customHeight="1">
+    <row r="6" spans="1:26" s="6" customFormat="1" ht="28" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="42"/>
       <c r="B6" s="21"/>
       <c r="C6" s="21"/>
@@ -1822,7 +1850,7 @@
       <c r="Y6" s="5"/>
       <c r="Z6" s="5"/>
     </row>
-    <row r="7" spans="1:26" s="6" customFormat="1" ht="28" customHeight="1">
+    <row r="7" spans="1:26" s="6" customFormat="1" ht="28" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="42"/>
       <c r="B7" s="21"/>
       <c r="C7" s="21"/>
@@ -1850,7 +1878,7 @@
       <c r="Y7" s="5"/>
       <c r="Z7" s="5"/>
     </row>
-    <row r="8" spans="1:26" s="6" customFormat="1" ht="28" customHeight="1">
+    <row r="8" spans="1:26" s="6" customFormat="1" ht="28" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="42"/>
       <c r="B8" s="21"/>
       <c r="C8" s="21"/>
@@ -1878,7 +1906,7 @@
       <c r="Y8" s="5"/>
       <c r="Z8" s="5"/>
     </row>
-    <row r="9" spans="1:26" s="6" customFormat="1" ht="28" customHeight="1">
+    <row r="9" spans="1:26" s="6" customFormat="1" ht="28" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="42"/>
       <c r="B9" s="21"/>
       <c r="C9" s="21"/>
@@ -1906,7 +1934,7 @@
       <c r="Y9" s="5"/>
       <c r="Z9" s="5"/>
     </row>
-    <row r="10" spans="1:26" s="6" customFormat="1" ht="28" customHeight="1">
+    <row r="10" spans="1:26" s="6" customFormat="1" ht="28" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="42"/>
       <c r="B10" s="21"/>
       <c r="C10" s="21"/>
@@ -1934,7 +1962,7 @@
       <c r="Y10" s="5"/>
       <c r="Z10" s="5"/>
     </row>
-    <row r="11" spans="1:26" s="6" customFormat="1" ht="28" customHeight="1">
+    <row r="11" spans="1:26" s="6" customFormat="1" ht="28" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="42"/>
       <c r="B11" s="21"/>
       <c r="C11" s="21"/>
@@ -1962,7 +1990,7 @@
       <c r="Y11" s="5"/>
       <c r="Z11" s="5"/>
     </row>
-    <row r="12" spans="1:26" s="8" customFormat="1" ht="28" customHeight="1" thickBot="1">
+    <row r="12" spans="1:26" s="8" customFormat="1" ht="28" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="43"/>
       <c r="B12" s="22"/>
       <c r="C12" s="22"/>
@@ -1990,7 +2018,7 @@
       <c r="Y12" s="7"/>
       <c r="Z12" s="7"/>
     </row>
-    <row r="13" spans="1:26" s="14" customFormat="1" ht="36" customHeight="1" thickBot="1">
+    <row r="13" spans="1:26" s="14" customFormat="1" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="17" t="s">
         <v>1</v>
       </c>
@@ -2020,7 +2048,7 @@
       <c r="Y13" s="13"/>
       <c r="Z13" s="13"/>
     </row>
-    <row r="14" spans="1:26" s="4" customFormat="1" ht="89" customHeight="1" thickBot="1">
+    <row r="14" spans="1:26" s="4" customFormat="1" ht="89" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="18" t="s">
         <v>4</v>
       </c>
@@ -2050,11 +2078,11 @@
       <c r="Y14" s="3"/>
       <c r="Z14" s="3"/>
     </row>
-    <row r="15" spans="1:26" ht="36" customHeight="1" thickBot="1">
+    <row r="15" spans="1:26" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B15" s="31"/>
       <c r="C15"/>
     </row>
-    <row r="16" spans="1:26" s="20" customFormat="1" ht="36" customHeight="1" thickBot="1">
+    <row r="16" spans="1:26" s="20" customFormat="1" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="19" t="s">
         <v>5</v>
       </c>
@@ -2069,63 +2097,63 @@
       <c r="J16" s="45"/>
       <c r="K16" s="45"/>
     </row>
-    <row r="18" spans="2:3">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B18" s="35"/>
       <c r="C18" s="36"/>
     </row>
-    <row r="19" spans="2:3">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B19" s="35"/>
       <c r="C19" s="35"/>
     </row>
-    <row r="20" spans="2:3">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B20" s="36"/>
       <c r="C20" s="36"/>
     </row>
-    <row r="21" spans="2:3">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B21" s="36"/>
       <c r="C21" s="36"/>
     </row>
-    <row r="22" spans="2:3">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B22" s="36"/>
       <c r="C22" s="36"/>
     </row>
-    <row r="23" spans="2:3">
+    <row r="23" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B23" s="36"/>
       <c r="C23" s="36"/>
     </row>
-    <row r="24" spans="2:3">
+    <row r="24" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B24" s="36"/>
       <c r="C24" s="36"/>
     </row>
-    <row r="25" spans="2:3">
+    <row r="25" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B25" s="36"/>
       <c r="C25" s="36"/>
     </row>
-    <row r="26" spans="2:3">
+    <row r="26" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B26" s="36"/>
       <c r="C26" s="36"/>
     </row>
-    <row r="27" spans="2:3">
+    <row r="27" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B27" s="36"/>
       <c r="C27" s="36"/>
     </row>
-    <row r="28" spans="2:3">
+    <row r="28" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B28" s="36"/>
       <c r="C28" s="36"/>
     </row>
-    <row r="29" spans="2:3">
+    <row r="29" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B29" s="36"/>
       <c r="C29" s="36"/>
     </row>
-    <row r="30" spans="2:3">
+    <row r="30" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B30" s="36"/>
       <c r="C30" s="36"/>
     </row>
-    <row r="31" spans="2:3">
+    <row r="31" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B31" s="36"/>
       <c r="C31" s="36"/>
     </row>
-    <row r="32" spans="2:3">
+    <row r="32" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B32" s="36"/>
       <c r="C32" s="36"/>
     </row>

</xml_diff>